<commit_message>
TODO: Generate non overlapping CCC constraint programatically
TODO: Work on reducing major electives

TODO: Work on room allottments
</commit_message>
<xml_diff>
--- a/COS.xlsx
+++ b/COS.xlsx
@@ -11,7 +11,8 @@
     <sheet name="Offered Course List" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Offered Course List'!$C$1:$C$307</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Offered Course List'!$A$1:$A$311</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Offered Course List'!$C$1:$C$307</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -4473,7 +4474,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4487,10 +4488,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4581,10 +4578,10 @@
   </sheetPr>
   <dimension ref="A1:BZ311"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AL1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A307" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="AL1" activeCellId="0" sqref="AL1"/>
-      <selection pane="bottomLeft" activeCell="AM308" activeCellId="0" sqref="AM308:AM311"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="66" zoomScaleNormal="66" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A199" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A200" activeCellId="0" sqref="A200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17234,7 +17231,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="209" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="209" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="1" t="s">
         <v>82</v>
       </c>
@@ -24303,437 +24300,437 @@
       </c>
     </row>
     <row r="308" customFormat="false" ht="70.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A308" s="5" t="s">
+      <c r="A308" s="4" t="s">
         <v>859</v>
       </c>
-      <c r="B308" s="5" t="s">
+      <c r="B308" s="4" t="s">
         <v>860</v>
       </c>
-      <c r="C308" s="5" t="s">
+      <c r="C308" s="4" t="s">
         <v>1257</v>
       </c>
-      <c r="D308" s="5" t="s">
+      <c r="D308" s="4" t="s">
         <v>1258</v>
       </c>
-      <c r="E308" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F308" s="5" t="s">
+      <c r="E308" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F308" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G308" s="5" t="s">
+      <c r="G308" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H308" s="5" t="s">
+      <c r="H308" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="I308" s="5" t="s">
+      <c r="I308" s="4" t="s">
         <v>864</v>
       </c>
-      <c r="J308" s="5" t="s">
+      <c r="J308" s="4" t="s">
         <v>865</v>
       </c>
-      <c r="K308" s="5"/>
-      <c r="L308" s="5"/>
-      <c r="M308" s="5"/>
-      <c r="N308" s="5"/>
-      <c r="O308" s="5"/>
-      <c r="P308" s="5"/>
-      <c r="Q308" s="5"/>
-      <c r="R308" s="5"/>
-      <c r="S308" s="5" t="n">
+      <c r="K308" s="4"/>
+      <c r="L308" s="4"/>
+      <c r="M308" s="4"/>
+      <c r="N308" s="4"/>
+      <c r="O308" s="4"/>
+      <c r="P308" s="4"/>
+      <c r="Q308" s="4"/>
+      <c r="R308" s="4"/>
+      <c r="S308" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="T308" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="U308" s="5"/>
-      <c r="V308" s="5"/>
-      <c r="W308" s="5" t="n">
+      <c r="T308" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="U308" s="4"/>
+      <c r="V308" s="4"/>
+      <c r="W308" s="4" t="n">
         <v>1.5</v>
       </c>
-      <c r="X308" s="5" t="s">
+      <c r="X308" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Y308" s="5"/>
-      <c r="Z308" s="5"/>
-      <c r="AA308" s="5" t="s">
+      <c r="Y308" s="4"/>
+      <c r="Z308" s="4"/>
+      <c r="AA308" s="4" t="s">
         <v>1114</v>
       </c>
-      <c r="AB308" s="5"/>
-      <c r="AC308" s="5"/>
-      <c r="AD308" s="5"/>
-      <c r="AE308" s="5"/>
-      <c r="AF308" s="5" t="s">
+      <c r="AB308" s="4"/>
+      <c r="AC308" s="4"/>
+      <c r="AD308" s="4"/>
+      <c r="AE308" s="4"/>
+      <c r="AF308" s="4" t="s">
         <v>1259</v>
       </c>
-      <c r="AG308" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH308" s="5"/>
-      <c r="AI308" s="5"/>
-      <c r="AJ308" s="5"/>
-      <c r="AK308" s="5"/>
-      <c r="AL308" s="5"/>
-      <c r="AM308" s="5" t="s">
+      <c r="AG308" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH308" s="4"/>
+      <c r="AI308" s="4"/>
+      <c r="AJ308" s="4"/>
+      <c r="AK308" s="4"/>
+      <c r="AL308" s="4"/>
+      <c r="AM308" s="4" t="s">
         <v>1115</v>
       </c>
-      <c r="AN308" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="AO308" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP308" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ308" s="5" t="s">
+      <c r="AN308" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO308" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP308" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ308" s="4" t="s">
         <v>1260</v>
       </c>
-      <c r="AR308" s="5"/>
-      <c r="AS308" s="5"/>
-      <c r="AT308" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="AU308" s="5" t="s">
+      <c r="AR308" s="4"/>
+      <c r="AS308" s="4"/>
+      <c r="AT308" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU308" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="AV308" s="5"/>
-      <c r="AW308" s="5"/>
-      <c r="AX308" s="5"/>
-      <c r="AY308" s="5"/>
-      <c r="AZ308" s="5"/>
-      <c r="BA308" s="5"/>
-      <c r="BB308" s="5"/>
-      <c r="BC308" s="5"/>
+      <c r="AV308" s="4"/>
+      <c r="AW308" s="4"/>
+      <c r="AX308" s="4"/>
+      <c r="AY308" s="4"/>
+      <c r="AZ308" s="4"/>
+      <c r="BA308" s="4"/>
+      <c r="BB308" s="4"/>
+      <c r="BC308" s="4"/>
     </row>
     <row r="309" customFormat="false" ht="83.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A309" s="5" t="s">
+      <c r="A309" s="4" t="s">
         <v>859</v>
       </c>
-      <c r="B309" s="5" t="s">
+      <c r="B309" s="4" t="s">
         <v>860</v>
       </c>
-      <c r="C309" s="5" t="s">
+      <c r="C309" s="4" t="s">
         <v>1261</v>
       </c>
-      <c r="D309" s="5" t="s">
+      <c r="D309" s="4" t="s">
         <v>1262</v>
       </c>
-      <c r="E309" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F309" s="5" t="s">
+      <c r="E309" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F309" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G309" s="5" t="s">
+      <c r="G309" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H309" s="5" t="s">
+      <c r="H309" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="I309" s="5"/>
-      <c r="J309" s="5"/>
-      <c r="K309" s="5"/>
-      <c r="L309" s="5"/>
-      <c r="M309" s="5"/>
-      <c r="N309" s="5"/>
-      <c r="O309" s="5"/>
-      <c r="P309" s="5"/>
-      <c r="Q309" s="5"/>
-      <c r="R309" s="5"/>
-      <c r="S309" s="5" t="n">
+      <c r="I309" s="4"/>
+      <c r="J309" s="4"/>
+      <c r="K309" s="4"/>
+      <c r="L309" s="4"/>
+      <c r="M309" s="4"/>
+      <c r="N309" s="4"/>
+      <c r="O309" s="4"/>
+      <c r="P309" s="4"/>
+      <c r="Q309" s="4"/>
+      <c r="R309" s="4"/>
+      <c r="S309" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="T309" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="U309" s="5"/>
-      <c r="V309" s="5"/>
-      <c r="W309" s="5" t="n">
+      <c r="T309" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="U309" s="4"/>
+      <c r="V309" s="4"/>
+      <c r="W309" s="4" t="n">
         <v>1.5</v>
       </c>
-      <c r="X309" s="5" t="s">
+      <c r="X309" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Y309" s="5"/>
-      <c r="Z309" s="5"/>
-      <c r="AA309" s="5" t="s">
+      <c r="Y309" s="4"/>
+      <c r="Z309" s="4"/>
+      <c r="AA309" s="4" t="s">
         <v>1263</v>
       </c>
-      <c r="AB309" s="5"/>
-      <c r="AC309" s="5"/>
-      <c r="AD309" s="5"/>
-      <c r="AE309" s="5"/>
-      <c r="AF309" s="5" t="s">
+      <c r="AB309" s="4"/>
+      <c r="AC309" s="4"/>
+      <c r="AD309" s="4"/>
+      <c r="AE309" s="4"/>
+      <c r="AF309" s="4" t="s">
         <v>1264</v>
       </c>
-      <c r="AG309" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH309" s="5"/>
-      <c r="AI309" s="5"/>
-      <c r="AJ309" s="5"/>
-      <c r="AK309" s="5"/>
-      <c r="AL309" s="5"/>
-      <c r="AM309" s="5" t="s">
+      <c r="AG309" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH309" s="4"/>
+      <c r="AI309" s="4"/>
+      <c r="AJ309" s="4"/>
+      <c r="AK309" s="4"/>
+      <c r="AL309" s="4"/>
+      <c r="AM309" s="4" t="s">
         <v>538</v>
       </c>
-      <c r="AN309" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="AO309" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP309" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ309" s="5" t="s">
+      <c r="AN309" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO309" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP309" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ309" s="4" t="s">
         <v>1265</v>
       </c>
-      <c r="AR309" s="5"/>
-      <c r="AS309" s="5"/>
-      <c r="AT309" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="AU309" s="5" t="s">
+      <c r="AR309" s="4"/>
+      <c r="AS309" s="4"/>
+      <c r="AT309" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU309" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="AV309" s="5"/>
-      <c r="AW309" s="5"/>
-      <c r="AX309" s="5"/>
-      <c r="AY309" s="5"/>
-      <c r="AZ309" s="5"/>
-      <c r="BA309" s="5"/>
-      <c r="BB309" s="5"/>
-      <c r="BC309" s="5"/>
+      <c r="AV309" s="4"/>
+      <c r="AW309" s="4"/>
+      <c r="AX309" s="4"/>
+      <c r="AY309" s="4"/>
+      <c r="AZ309" s="4"/>
+      <c r="BA309" s="4"/>
+      <c r="BB309" s="4"/>
+      <c r="BC309" s="4"/>
     </row>
     <row r="310" customFormat="false" ht="70.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A310" s="5" t="s">
+      <c r="A310" s="4" t="s">
         <v>859</v>
       </c>
-      <c r="B310" s="5" t="s">
+      <c r="B310" s="4" t="s">
         <v>860</v>
       </c>
-      <c r="C310" s="5" t="s">
+      <c r="C310" s="4" t="s">
         <v>1266</v>
       </c>
-      <c r="D310" s="5" t="s">
+      <c r="D310" s="4" t="s">
         <v>1267</v>
       </c>
-      <c r="E310" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F310" s="5" t="s">
+      <c r="E310" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F310" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G310" s="5" t="s">
+      <c r="G310" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H310" s="5" t="s">
+      <c r="H310" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="I310" s="5"/>
-      <c r="J310" s="5"/>
-      <c r="K310" s="5"/>
-      <c r="L310" s="5"/>
-      <c r="M310" s="5"/>
-      <c r="N310" s="5"/>
-      <c r="O310" s="5"/>
-      <c r="P310" s="5"/>
-      <c r="Q310" s="5"/>
-      <c r="R310" s="5"/>
-      <c r="S310" s="5" t="n">
+      <c r="I310" s="4"/>
+      <c r="J310" s="4"/>
+      <c r="K310" s="4"/>
+      <c r="L310" s="4"/>
+      <c r="M310" s="4"/>
+      <c r="N310" s="4"/>
+      <c r="O310" s="4"/>
+      <c r="P310" s="4"/>
+      <c r="Q310" s="4"/>
+      <c r="R310" s="4"/>
+      <c r="S310" s="4" t="n">
         <v>45</v>
       </c>
-      <c r="T310" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="U310" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="V310" s="5"/>
-      <c r="W310" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="X310" s="5" t="s">
+      <c r="T310" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="U310" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="V310" s="4"/>
+      <c r="W310" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="X310" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Y310" s="5" t="s">
+      <c r="Y310" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="Z310" s="5"/>
-      <c r="AA310" s="5" t="s">
+      <c r="Z310" s="4"/>
+      <c r="AA310" s="4" t="s">
         <v>1268</v>
       </c>
-      <c r="AB310" s="5" t="s">
+      <c r="AB310" s="4" t="s">
         <v>1268</v>
       </c>
-      <c r="AC310" s="5"/>
-      <c r="AD310" s="5"/>
-      <c r="AE310" s="5"/>
-      <c r="AF310" s="5" t="s">
+      <c r="AC310" s="4"/>
+      <c r="AD310" s="4"/>
+      <c r="AE310" s="4"/>
+      <c r="AF310" s="4" t="s">
         <v>1269</v>
       </c>
-      <c r="AG310" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH310" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="AI310" s="5"/>
-      <c r="AJ310" s="5"/>
-      <c r="AK310" s="5"/>
-      <c r="AL310" s="5"/>
-      <c r="AM310" s="5" t="s">
+      <c r="AG310" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH310" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI310" s="4"/>
+      <c r="AJ310" s="4"/>
+      <c r="AK310" s="4"/>
+      <c r="AL310" s="4"/>
+      <c r="AM310" s="4" t="s">
         <v>1270</v>
       </c>
-      <c r="AN310" s="5" t="n">
+      <c r="AN310" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="AO310" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP310" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ310" s="5" t="s">
+      <c r="AO310" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP310" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ310" s="4" t="s">
         <v>1271</v>
       </c>
-      <c r="AR310" s="5"/>
-      <c r="AS310" s="5"/>
-      <c r="AT310" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="AU310" s="5" t="s">
+      <c r="AR310" s="4"/>
+      <c r="AS310" s="4"/>
+      <c r="AT310" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU310" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="AV310" s="5"/>
-      <c r="AW310" s="5"/>
-      <c r="AX310" s="5"/>
-      <c r="AY310" s="5"/>
-      <c r="AZ310" s="5"/>
-      <c r="BA310" s="5"/>
-      <c r="BB310" s="5"/>
-      <c r="BC310" s="5"/>
+      <c r="AV310" s="4"/>
+      <c r="AW310" s="4"/>
+      <c r="AX310" s="4"/>
+      <c r="AY310" s="4"/>
+      <c r="AZ310" s="4"/>
+      <c r="BA310" s="4"/>
+      <c r="BB310" s="4"/>
+      <c r="BC310" s="4"/>
     </row>
     <row r="311" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A311" s="5" t="s">
+      <c r="A311" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B311" s="5" t="s">
+      <c r="B311" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C311" s="5" t="s">
+      <c r="C311" s="4" t="s">
         <v>1272</v>
       </c>
-      <c r="D311" s="5" t="s">
+      <c r="D311" s="4" t="s">
         <v>1273</v>
       </c>
-      <c r="E311" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F311" s="5" t="s">
+      <c r="E311" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F311" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G311" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H311" s="5" t="s">
+      <c r="G311" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H311" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="I311" s="5" t="s">
+      <c r="I311" s="4" t="s">
         <v>828</v>
       </c>
-      <c r="J311" s="5"/>
-      <c r="K311" s="5"/>
-      <c r="L311" s="5"/>
-      <c r="M311" s="5"/>
-      <c r="N311" s="5"/>
-      <c r="O311" s="5"/>
-      <c r="P311" s="5"/>
-      <c r="Q311" s="5"/>
-      <c r="R311" s="5"/>
-      <c r="S311" s="5" t="n">
+      <c r="J311" s="4"/>
+      <c r="K311" s="4"/>
+      <c r="L311" s="4"/>
+      <c r="M311" s="4"/>
+      <c r="N311" s="4"/>
+      <c r="O311" s="4"/>
+      <c r="P311" s="4"/>
+      <c r="Q311" s="4"/>
+      <c r="R311" s="4"/>
+      <c r="S311" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="T311" s="5" t="n">
+      <c r="T311" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="U311" s="5"/>
-      <c r="V311" s="5" t="n">
+      <c r="U311" s="4"/>
+      <c r="V311" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="W311" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="X311" s="5" t="s">
+      <c r="W311" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="X311" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Y311" s="5"/>
-      <c r="Z311" s="5" t="s">
+      <c r="Y311" s="4"/>
+      <c r="Z311" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="AA311" s="5" t="s">
+      <c r="AA311" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="AB311" s="5"/>
-      <c r="AC311" s="5" t="s">
+      <c r="AB311" s="4"/>
+      <c r="AC311" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="AD311" s="5" t="s">
+      <c r="AD311" s="4" t="s">
         <v>877</v>
       </c>
-      <c r="AE311" s="5" t="n">
+      <c r="AE311" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AF311" s="5"/>
-      <c r="AG311" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH311" s="5"/>
-      <c r="AI311" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ311" s="5"/>
-      <c r="AK311" s="5"/>
-      <c r="AL311" s="5"/>
-      <c r="AM311" s="5" t="s">
+      <c r="AF311" s="4"/>
+      <c r="AG311" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH311" s="4"/>
+      <c r="AI311" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ311" s="4"/>
+      <c r="AK311" s="4"/>
+      <c r="AL311" s="4"/>
+      <c r="AM311" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="AN311" s="5" t="n">
+      <c r="AN311" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="AO311" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP311" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ311" s="5" t="s">
+      <c r="AO311" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP311" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ311" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="AR311" s="5"/>
-      <c r="AS311" s="5" t="s">
+      <c r="AR311" s="4"/>
+      <c r="AS311" s="4" t="s">
         <v>1274</v>
       </c>
-      <c r="AT311" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="AU311" s="5" t="s">
+      <c r="AT311" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU311" s="4" t="s">
         <v>804</v>
       </c>
-      <c r="AV311" s="5"/>
-      <c r="AW311" s="5"/>
-      <c r="AX311" s="5"/>
-      <c r="AY311" s="5"/>
-      <c r="AZ311" s="5"/>
-      <c r="BA311" s="5"/>
-      <c r="BB311" s="5"/>
-      <c r="BC311" s="5"/>
+      <c r="AV311" s="4"/>
+      <c r="AW311" s="4"/>
+      <c r="AX311" s="4"/>
+      <c r="AY311" s="4"/>
+      <c r="AZ311" s="4"/>
+      <c r="BA311" s="4"/>
+      <c r="BB311" s="4"/>
+      <c r="BC311" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C307"/>
+  <autoFilter ref="A1:A311"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>